<commit_message>
Add table of team total stats and player detail stats
</commit_message>
<xml_diff>
--- a/results/LSU_WR_2012-2022_TEST.xlsx
+++ b/results/LSU_WR_2012-2022_TEST.xlsx
@@ -14,27 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Data</t>
+    <t>YEAR</t>
   </si>
   <si>
-    <t>Geeks</t>
+    <t>Yards</t>
   </si>
   <si>
-    <t>For</t>
+    <t>TDs</t>
   </si>
   <si>
-    <t>geeks</t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>portal</t>
-  </si>
-  <si>
-    <t>for</t>
+    <t>GS</t>
   </si>
 </sst>
 </file>
@@ -392,71 +383,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2">
+        <v>2012</v>
+      </c>
+      <c r="C2">
+        <v>2316</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3">
+        <v>2013</v>
+      </c>
+      <c r="C3">
+        <v>1911</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4">
+        <v>2014</v>
+      </c>
+      <c r="C4">
+        <v>4862</v>
+      </c>
+      <c r="D4">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5">
+        <v>4000</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6">
+        <v>2016</v>
+      </c>
+      <c r="C6">
+        <v>3812</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7">
+        <v>2017</v>
+      </c>
+      <c r="C7">
+        <v>2039</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
+      <c r="B8">
+        <v>2018</v>
+      </c>
+      <c r="C8">
+        <v>2588</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2019</v>
+      </c>
+      <c r="C9">
+        <v>3691</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10">
+        <v>4449</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+      <c r="C11">
+        <v>5476</v>
+      </c>
+      <c r="D11">
+        <v>38</v>
+      </c>
+      <c r="E11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2022</v>
+      </c>
+      <c r="C12">
+        <v>4593</v>
+      </c>
+      <c r="D12">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>